<commit_message>
update test regression data
</commit_message>
<xml_diff>
--- a/tests/regression_data_windows/design_optimization_windows.xlsx
+++ b/tests/regression_data_windows/design_optimization_windows.xlsx
@@ -725,7 +725,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:ED5"/>
+  <dimension ref="A1:EE5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1399,6 +1399,11 @@
           <t>blockage</t>
         </is>
       </c>
+      <c r="EE1" s="1" t="inlineStr">
+        <is>
+          <t>h_is</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -1807,6 +1812,11 @@
           <t>b''</t>
         </is>
       </c>
+      <c r="EE2" t="inlineStr">
+        <is>
+          <t>b''</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -2198,6 +2208,9 @@
       </c>
       <c r="ED3" t="n">
         <v>0</v>
+      </c>
+      <c r="EE3" t="n">
+        <v>490189.7099025669</v>
       </c>
     </row>
     <row r="4">
@@ -2575,6 +2588,7 @@
       <c r="EB4" t="inlineStr"/>
       <c r="EC4" t="inlineStr"/>
       <c r="ED4" t="inlineStr"/>
+      <c r="EE4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -2966,6 +2980,9 @@
       </c>
       <c r="ED5" t="n">
         <v>0</v>
+      </c>
+      <c r="EE5" t="n">
+        <v>474663.510268038</v>
       </c>
     </row>
   </sheetData>
@@ -2979,7 +2996,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:ER3"/>
+  <dimension ref="A1:EN3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3690,37 +3707,17 @@
       </c>
       <c r="EL1" s="1" t="inlineStr">
         <is>
+          <t>h_is_throat</t>
+        </is>
+      </c>
+      <c r="EM1" s="1" t="inlineStr">
+        <is>
           <t>dh_s</t>
         </is>
       </c>
-      <c r="EM1" s="1" t="inlineStr">
+      <c r="EN1" s="1" t="inlineStr">
         <is>
           <t>incidence</t>
-        </is>
-      </c>
-      <c r="EN1" s="1" t="inlineStr">
-        <is>
-          <t>efficiency_drop_profile</t>
-        </is>
-      </c>
-      <c r="EO1" s="1" t="inlineStr">
-        <is>
-          <t>efficiency_drop_incidence</t>
-        </is>
-      </c>
-      <c r="EP1" s="1" t="inlineStr">
-        <is>
-          <t>efficiency_drop_secondary</t>
-        </is>
-      </c>
-      <c r="EQ1" s="1" t="inlineStr">
-        <is>
-          <t>efficiency_drop_clearance</t>
-        </is>
-      </c>
-      <c r="ER1" s="1" t="inlineStr">
-        <is>
-          <t>efficiency_drop_trailing</t>
         </is>
       </c>
     </row>
@@ -4137,25 +4134,13 @@
         <v>0</v>
       </c>
       <c r="EL2" t="n">
+        <v>490646.156185923</v>
+      </c>
+      <c r="EM2" t="n">
         <v>446.8077670247294</v>
       </c>
-      <c r="EM2" t="n">
+      <c r="EN2" t="n">
         <v>-20.45665123722149</v>
-      </c>
-      <c r="EN2" t="n">
-        <v>0.005059829407177755</v>
-      </c>
-      <c r="EO2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EP2" t="n">
-        <v>0.01072733292376794</v>
-      </c>
-      <c r="EQ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="ER2" t="n">
-        <v>0.002995745518082173</v>
       </c>
     </row>
     <row r="3">
@@ -4571,25 +4556,13 @@
         <v>0</v>
       </c>
       <c r="EL3" t="n">
+        <v>478710.3421281012</v>
+      </c>
+      <c r="EM3" t="n">
         <v>985.5562162786955</v>
       </c>
-      <c r="EM3" t="n">
+      <c r="EN3" t="n">
         <v>-51.59248076169214</v>
-      </c>
-      <c r="EN3" t="n">
-        <v>0.01700907330548201</v>
-      </c>
-      <c r="EO3" t="n">
-        <v>0</v>
-      </c>
-      <c r="EP3" t="n">
-        <v>0.004721882393046286</v>
-      </c>
-      <c r="EQ3" t="n">
-        <v>0.01362092236644145</v>
-      </c>
-      <c r="ER3" t="n">
-        <v>0.006078940637371107</v>
       </c>
     </row>
   </sheetData>
@@ -4698,182 +4671,182 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>stagger_angle</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>leading_edge_diameter</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>leading_edge_wedge_angle</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>trailing_edge_thickness</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>tip_clearance</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>throat_location_fraction</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>number_of_stages</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>number_of_cascades</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>axial_chord</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>radius_mean_in</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>radius_mean_out</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>radius_mean_throat</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>radius_hub_throat</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>radius_tip_throat</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>radius_shroud_in</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>radius_shroud_out</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>radius_shroud_throat</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>hub_tip_ratio_in</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>hub_tip_ratio_out</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>hub_tip_ratio_throat</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>A_in</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>A_out</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>A_throat</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>height</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>height_in</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>height_throat</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>height_out</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>flaring_angle</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>aspect_ratio</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>pitch_chord_ratio</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>solidity</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>maximum_thickness_chord_ratio</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>trailing_edge_thickness_opening_ratio</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>tip_clearance_height_ratio</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>leading_edge_diameter_chord_ratio</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
           <t>gauging_angle</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>stagger_angle</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>leading_edge_diameter</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>leading_edge_wedge_angle</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>trailing_edge_thickness</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>tip_clearance</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>throat_location_fraction</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>number_of_stages</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>number_of_cascades</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>axial_chord</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>radius_mean_in</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>radius_mean_out</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>radius_mean_throat</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>radius_hub_throat</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>radius_tip_throat</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>radius_shroud_in</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>radius_shroud_out</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>radius_shroud_throat</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>hub_tip_ratio_in</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>hub_tip_ratio_out</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>hub_tip_ratio_throat</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>A_in</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>A_out</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>A_throat</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>height</t>
-        </is>
-      </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>height_in</t>
-        </is>
-      </c>
-      <c r="AL1" s="1" t="inlineStr">
-        <is>
-          <t>height_throat</t>
-        </is>
-      </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>height_out</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>flaring_angle</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>aspect_ratio</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>pitch_chord_ratio</t>
-        </is>
-      </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>solidity</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>maximum_thickness_chord_ratio</t>
-        </is>
-      </c>
-      <c r="AS1" s="1" t="inlineStr">
-        <is>
-          <t>trailing_edge_thickness_opening_ratio</t>
-        </is>
-      </c>
-      <c r="AT1" s="1" t="inlineStr">
-        <is>
-          <t>tip_clearance_height_ratio</t>
-        </is>
-      </c>
-      <c r="AU1" s="1" t="inlineStr">
-        <is>
-          <t>leading_edge_diameter_chord_ratio</t>
         </is>
       </c>
     </row>
@@ -4914,112 +4887,112 @@
         <v>20.45665123722149</v>
       </c>
       <c r="L2" t="n">
-        <v>79.19999999999996</v>
+        <v>-29.37167438138923</v>
       </c>
       <c r="M2" t="n">
-        <v>-29.37167438138923</v>
+        <v>0.01200896</v>
       </c>
       <c r="N2" t="n">
-        <v>0.01200896</v>
+        <v>45</v>
       </c>
       <c r="O2" t="n">
-        <v>45</v>
+        <v>7.298042391729463e-05</v>
       </c>
       <c r="P2" t="n">
-        <v>7.298042391729463e-05</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2" t="n">
         <v>1</v>
       </c>
       <c r="S2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T2" t="n">
-        <v>2</v>
+        <v>0.009050956839588991</v>
       </c>
       <c r="U2" t="n">
-        <v>0.009050956839588991</v>
+        <v>0.04671098227814975</v>
       </c>
       <c r="V2" t="n">
-        <v>0.04671098227814975</v>
+        <v>0.04671098227814976</v>
       </c>
       <c r="W2" t="n">
         <v>0.04671098227814976</v>
       </c>
       <c r="X2" t="n">
-        <v>0.04671098227814976</v>
+        <v>0.03847862738741641</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.03847862738741641</v>
+        <v>0.0549433371688831</v>
       </c>
       <c r="Z2" t="n">
+        <v>0.05838872784768715</v>
+      </c>
+      <c r="AA2" t="n">
         <v>0.0549433371688831</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0.05838872784768715</v>
       </c>
       <c r="AB2" t="n">
         <v>0.0549433371688831</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.0549433371688831</v>
+        <v>0.6000000000000012</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.6000000000000012</v>
+        <v>0.7003329133274525</v>
       </c>
       <c r="AE2" t="n">
         <v>0.7003329133274525</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.7003329133274525</v>
+        <v>0.006854690853459023</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.006854690853459023</v>
+        <v>0.004832289540469407</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.004832289540469407</v>
+        <v>0.0009054807665520083</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.0009054807665520083</v>
+        <v>0.01991010046027074</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.01991010046027074</v>
+        <v>0.02335549113907479</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.02335549113907479</v>
+        <v>0.01646470978146669</v>
       </c>
       <c r="AL2" t="n">
         <v>0.01646470978146669</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.01646470978146669</v>
+        <v>-20.84012299640998</v>
       </c>
       <c r="AN2" t="n">
-        <v>-20.84012299640998</v>
+        <v>1.917011061422102</v>
       </c>
       <c r="AO2" t="n">
-        <v>1.917011061422102</v>
+        <v>0.75</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.75</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="AQ2" t="n">
-        <v>1.333333333333333</v>
+        <v>0.2245708140465268</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.2245708140465268</v>
+        <v>0.05000000000000031</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.05000000000000031</v>
+        <v>0</v>
       </c>
       <c r="AT2" t="n">
-        <v>0</v>
+        <v>1.15626283263176</v>
       </c>
       <c r="AU2" t="n">
-        <v>1.15626283263176</v>
+        <v>79.19999999999996</v>
       </c>
     </row>
     <row r="3">
@@ -5059,108 +5032,108 @@
         <v>-20.3418464234055</v>
       </c>
       <c r="L3" t="n">
-        <v>-78.9865367125031</v>
+        <v>29.3223451445488</v>
       </c>
       <c r="M3" t="n">
-        <v>29.3223451445488</v>
+        <v>0.01200896</v>
       </c>
       <c r="N3" t="n">
-        <v>0.01200896</v>
+        <v>45</v>
       </c>
       <c r="O3" t="n">
-        <v>45</v>
+        <v>6.02395522800882e-05</v>
       </c>
       <c r="P3" t="n">
-        <v>6.02395522800882e-05</v>
+        <v>0.0005</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="R3" t="n">
         <v>1</v>
       </c>
+      <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
+      <c r="T3" t="n">
+        <v>0.007331331261925708</v>
+      </c>
       <c r="U3" t="n">
-        <v>0.007331331261925708</v>
+        <v>0.04671098227814977</v>
       </c>
       <c r="V3" t="n">
-        <v>0.04671098227814977</v>
+        <v>0.04671098227814975</v>
       </c>
       <c r="W3" t="n">
         <v>0.04671098227814975</v>
       </c>
       <c r="X3" t="n">
-        <v>0.04671098227814975</v>
+        <v>0.03812972904352323</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.03812972904352323</v>
+        <v>0.05529223551277628</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.05529223551277628</v>
+        <v>0.05544333716887227</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.05544333716887227</v>
+        <v>0.05579223551277628</v>
       </c>
       <c r="AB3" t="n">
         <v>0.05579223551277628</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.05579223551277628</v>
+        <v>0.7003329133277881</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.7003329133277881</v>
+        <v>0.6896036792491896</v>
       </c>
       <c r="AE3" t="n">
         <v>0.6896036792491896</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.6896036792491896</v>
+        <v>0.004832289540463043</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.004832289540463043</v>
+        <v>0.005037088512362603</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.005037088512362603</v>
+        <v>0.0009622836343852729</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.0009622836343852729</v>
+        <v>0.01681360812534903</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.01681360812534903</v>
+        <v>0.01646470978144501</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.01646470978144501</v>
+        <v>0.01716250646925305</v>
       </c>
       <c r="AL3" t="n">
         <v>0.01716250646925305</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.01716250646925305</v>
+        <v>2.724652705685985</v>
       </c>
       <c r="AN3" t="n">
-        <v>2.724652705685985</v>
+        <v>1.999557838150698</v>
       </c>
       <c r="AO3" t="n">
-        <v>1.999557838150698</v>
+        <v>0.7500000000000001</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.7500000000000001</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="AQ3" t="n">
-        <v>1.333333333333333</v>
+        <v>0.2241604789198857</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.2241604789198857</v>
+        <v>0.05000000000000016</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.05000000000000016</v>
+        <v>0.02973781690832768</v>
       </c>
       <c r="AT3" t="n">
-        <v>0.02973781690832768</v>
+        <v>1.42816520505409</v>
       </c>
       <c r="AU3" t="n">
-        <v>1.42816520505409</v>
+        <v>-78.9865367125031</v>
       </c>
     </row>
   </sheetData>

</xml_diff>